<commit_message>
add more features to the texh table
</commit_message>
<xml_diff>
--- a/Documentations/Features-Garrett.xlsx
+++ b/Documentations/Features-Garrett.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="200" yWindow="280" windowWidth="14380" windowHeight="16640" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="200" yWindow="280" windowWidth="26780" windowHeight="16640" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="193">
   <si>
     <t>REQUIRED</t>
   </si>
@@ -146,9 +146,6 @@
     <t>iPhone (iOS)</t>
   </si>
   <si>
-    <t>Other (Android)</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
@@ -188,9 +185,6 @@
     <t>Can be powered by coin cell</t>
   </si>
   <si>
-    <t>Robustness</t>
-  </si>
-  <si>
     <t>Strong</t>
   </si>
   <si>
@@ -218,18 +212,12 @@
     <t>Cost</t>
   </si>
   <si>
-    <t>Good</t>
-  </si>
-  <si>
     <t>iPhone integration</t>
   </si>
   <si>
     <t>Android integration</t>
   </si>
   <si>
-    <t>Tablet</t>
-  </si>
-  <si>
     <t>battery charge indicator</t>
   </si>
   <si>
@@ -512,12 +500,6 @@
     <t xml:space="preserve">Must not exceed 1 pound </t>
   </si>
   <si>
-    <t>Dry electrode [3][4]</t>
-  </si>
-  <si>
-    <t>IR receiver/transmitter [5]</t>
-  </si>
-  <si>
     <t>Bluetooth [6]</t>
   </si>
   <si>
@@ -561,6 +543,63 @@
   </si>
   <si>
     <t>Mio Alpha [18]</t>
+  </si>
+  <si>
+    <t>Samasung Galaxy Gear</t>
+  </si>
+  <si>
+    <t>Phone (Android)</t>
+  </si>
+  <si>
+    <t>Tablet (Andoid)</t>
+  </si>
+  <si>
+    <t>iPad (IOS)</t>
+  </si>
+  <si>
+    <t>Windows phone (Windows 8)</t>
+  </si>
+  <si>
+    <t>Windows table (Windows 8)</t>
+  </si>
+  <si>
+    <t>E-ink Display</t>
+  </si>
+  <si>
+    <t>Wifi</t>
+  </si>
+  <si>
+    <t>Zigbee 2.4 Ghz</t>
+  </si>
+  <si>
+    <t>Dry electrode (ECG) [3][4]</t>
+  </si>
+  <si>
+    <t>IR receiver/transmitter (PPG) [5]</t>
+  </si>
+  <si>
+    <t>600 Mb/s</t>
+  </si>
+  <si>
+    <t>NFC</t>
+  </si>
+  <si>
+    <t>424 KP/s</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Easily affected by interferance</t>
+  </si>
+  <si>
+    <t>Up to 92m</t>
+  </si>
+  <si>
+    <t>Less than 11 cm</t>
+  </si>
+  <si>
+    <t>Yes (some)</t>
   </si>
 </sst>
 </file>
@@ -1289,7 +1328,7 @@
     <row r="16" spans="2:4" ht="20">
       <c r="B16" s="16"/>
       <c r="C16" s="16" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D16" s="16" t="s">
         <v>24</v>
@@ -1320,12 +1359,11 @@
       <c r="B20" s="16"/>
       <c r="C20" s="16"/>
       <c r="D20" s="16" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1336,10 +1374,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:Q31"/>
+  <dimension ref="B4:Q39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1363,19 +1401,19 @@
         <v>34</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E4" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="G4" s="5" t="s">
         <v>48</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>49</v>
       </c>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
@@ -1390,22 +1428,22 @@
     </row>
     <row r="5" spans="2:17">
       <c r="B5" s="6" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
       <c r="C5" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>44</v>
-      </c>
       <c r="E5" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -1420,22 +1458,22 @@
     </row>
     <row r="6" spans="2:17">
       <c r="B6" s="6" t="s">
-        <v>164</v>
+        <v>184</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -1453,37 +1491,37 @@
         <v>35</v>
       </c>
       <c r="C7" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>51</v>
-      </c>
       <c r="E7" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F7" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="G7" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="G7" s="5" t="s">
-        <v>57</v>
-      </c>
       <c r="H7" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="I7" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="J7" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K7" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="J7" s="5" t="s">
+      <c r="L7" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="K7" s="5" t="s">
+      <c r="M7" s="5" t="s">
         <v>64</v>
-      </c>
-      <c r="L7" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="M7" s="5" t="s">
-        <v>67</v>
       </c>
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
@@ -1492,40 +1530,40 @@
     </row>
     <row r="8" spans="2:17">
       <c r="B8" s="6" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F8" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="G8" s="6" t="s">
-        <v>58</v>
-      </c>
       <c r="H8" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>65</v>
+        <v>188</v>
       </c>
       <c r="L8" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M8" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N8" s="3"/>
       <c r="O8" s="3"/>
@@ -1534,77 +1572,75 @@
     </row>
     <row r="9" spans="2:17">
       <c r="B9" s="6" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M9" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
       <c r="P9" s="3"/>
       <c r="Q9" s="3"/>
     </row>
-    <row r="10" spans="2:17" ht="43" customHeight="1">
-      <c r="B10" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="J10" s="5" t="s">
-        <v>79</v>
-      </c>
+    <row r="10" spans="2:17">
+      <c r="B10" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
       <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
+      <c r="L10" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="M10" s="6" t="s">
+        <v>42</v>
+      </c>
       <c r="N10" s="3"/>
       <c r="O10" s="3"/>
       <c r="P10" s="3"/>
@@ -1612,35 +1648,33 @@
     </row>
     <row r="11" spans="2:17">
       <c r="B11" s="6" t="s">
-        <v>167</v>
+        <v>186</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>75</v>
+        <v>42</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>72</v>
+        <v>187</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>74</v>
+        <v>42</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="H11" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="I11" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="J11" s="6" t="s">
-        <v>46</v>
-      </c>
+        <v>191</v>
+      </c>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
       <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
+      <c r="L11" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="M11" s="6" t="s">
+        <v>192</v>
+      </c>
       <c r="N11" s="3"/>
       <c r="O11" s="3"/>
       <c r="P11" s="3"/>
@@ -1648,67 +1682,59 @@
     </row>
     <row r="12" spans="2:17">
       <c r="B12" s="6" t="s">
-        <v>168</v>
+        <v>182</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>81</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
       <c r="F12" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="H12" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="I12" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="J12" s="6" t="s">
-        <v>72</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
       <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
+      <c r="L12" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="M12" s="6" t="s">
+        <v>41</v>
+      </c>
       <c r="N12" s="3"/>
       <c r="O12" s="3"/>
       <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
     </row>
-    <row r="13" spans="2:17">
-      <c r="B13" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="D13" s="6" t="s">
+    <row r="13" spans="2:17" ht="43" customHeight="1">
+      <c r="B13" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="G13" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="E13" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="I13" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="J13" s="6" t="s">
-        <v>72</v>
+      <c r="H13" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>75</v>
       </c>
       <c r="K13" s="6"/>
       <c r="L13" s="6"/>
@@ -1720,31 +1746,31 @@
     </row>
     <row r="14" spans="2:17">
       <c r="B14" s="6" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>72</v>
+        <v>45</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="H14" s="6" t="s">
         <v>42</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>72</v>
+        <v>45</v>
       </c>
       <c r="K14" s="6"/>
       <c r="L14" s="6"/>
@@ -1754,32 +1780,34 @@
       <c r="P14" s="3"/>
       <c r="Q14" s="3"/>
     </row>
-    <row r="15" spans="2:17" ht="43" customHeight="1">
-      <c r="B15" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="I15" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="J15" s="6"/>
+    <row r="15" spans="2:17">
+      <c r="B15" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="J15" s="6" t="s">
+        <v>68</v>
+      </c>
       <c r="K15" s="6"/>
       <c r="L15" s="6"/>
       <c r="M15" s="6"/>
@@ -1790,30 +1818,32 @@
     </row>
     <row r="16" spans="2:17">
       <c r="B16" s="6" t="s">
-        <v>169</v>
+        <v>76</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="G16" s="8">
-        <v>10</v>
+        <v>77</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>68</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>89</v>
+        <v>41</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="J16" s="6"/>
+        <v>42</v>
+      </c>
+      <c r="J16" s="6" t="s">
+        <v>68</v>
+      </c>
       <c r="K16" s="6"/>
       <c r="L16" s="6"/>
       <c r="M16" s="6"/>
@@ -1824,30 +1854,32 @@
     </row>
     <row r="17" spans="2:17">
       <c r="B17" s="6" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>91</v>
+        <v>68</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="G17" s="8">
-        <v>40</v>
+        <v>68</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>68</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>89</v>
+        <v>41</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="J17" s="6"/>
+        <v>42</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>68</v>
+      </c>
       <c r="K17" s="6"/>
       <c r="L17" s="6"/>
       <c r="M17" s="6"/>
@@ -1856,30 +1888,30 @@
       <c r="P17" s="3"/>
       <c r="Q17" s="3"/>
     </row>
-    <row r="18" spans="2:17">
-      <c r="B18" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="C18" s="6" t="s">
+    <row r="18" spans="2:17" ht="43" customHeight="1">
+      <c r="B18" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F18" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="D18" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="G18" s="8">
-        <v>30</v>
-      </c>
-      <c r="H18" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="I18" s="6" t="s">
-        <v>100</v>
+      <c r="G18" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>91</v>
       </c>
       <c r="J18" s="6"/>
       <c r="K18" s="6"/>
@@ -1890,25 +1922,31 @@
       <c r="P18" s="3"/>
       <c r="Q18" s="3"/>
     </row>
-    <row r="19" spans="2:17" ht="43" customHeight="1">
-      <c r="B19" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
+    <row r="19" spans="2:17">
+      <c r="B19" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="G19" s="8">
+        <v>10</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>92</v>
+      </c>
       <c r="J19" s="6"/>
       <c r="K19" s="6"/>
       <c r="L19" s="6"/>
@@ -1920,23 +1958,29 @@
     </row>
     <row r="20" spans="2:17">
       <c r="B20" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="G20" s="8">
         <v>40</v>
       </c>
-      <c r="C20" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
+      <c r="H20" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>90</v>
+      </c>
       <c r="J20" s="6"/>
       <c r="K20" s="6"/>
       <c r="L20" s="6"/>
@@ -1948,21 +1992,13 @@
     </row>
     <row r="21" spans="2:17">
       <c r="B21" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G21" s="6"/>
+        <v>180</v>
+      </c>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="8"/>
       <c r="H21" s="6"/>
       <c r="I21" s="6"/>
       <c r="J21" s="6"/>
@@ -1976,23 +2012,29 @@
     </row>
     <row r="22" spans="2:17">
       <c r="B22" s="6" t="s">
-        <v>68</v>
+        <v>165</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>43</v>
+        <v>80</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>43</v>
+        <v>89</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>43</v>
+        <v>93</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
+        <v>94</v>
+      </c>
+      <c r="G22" s="8">
+        <v>30</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="I22" s="6" t="s">
+        <v>96</v>
+      </c>
       <c r="J22" s="6"/>
       <c r="K22" s="6"/>
       <c r="L22" s="6"/>
@@ -2004,35 +2046,25 @@
     </row>
     <row r="23" spans="2:17" ht="43" customHeight="1">
       <c r="B23" s="4" t="s">
-        <v>114</v>
+        <v>38</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>117</v>
+        <v>97</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>115</v>
+        <v>98</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="G23" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="H23" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="I23" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="J23" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="K23" s="5" t="s">
-        <v>118</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
       <c r="L23" s="6"/>
       <c r="M23" s="6"/>
       <c r="N23" s="3"/>
@@ -2042,35 +2074,25 @@
     </row>
     <row r="24" spans="2:17">
       <c r="B24" s="6" t="s">
-        <v>173</v>
+        <v>40</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>42</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>108</v>
+        <v>42</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G24" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="H24" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="I24" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="J24" s="8">
-        <v>130</v>
-      </c>
-      <c r="K24" s="6" t="s">
-        <v>43</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
       <c r="L24" s="6"/>
       <c r="M24" s="6"/>
       <c r="N24" s="3"/>
@@ -2079,247 +2101,454 @@
       <c r="Q24" s="3"/>
     </row>
     <row r="25" spans="2:17">
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
+      <c r="K25" s="6"/>
+      <c r="L25" s="6"/>
+      <c r="M25" s="6"/>
+      <c r="N25" s="3"/>
+      <c r="O25" s="3"/>
+      <c r="P25" s="3"/>
+      <c r="Q25" s="3"/>
+    </row>
+    <row r="26" spans="2:17">
+      <c r="B26" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6"/>
+      <c r="L26" s="6"/>
+      <c r="M26" s="6"/>
+      <c r="N26" s="3"/>
+      <c r="O26" s="3"/>
+      <c r="P26" s="3"/>
+      <c r="Q26" s="3"/>
+    </row>
+    <row r="27" spans="2:17">
+      <c r="B27" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6"/>
+      <c r="K27" s="6"/>
+      <c r="L27" s="6"/>
+      <c r="M27" s="6"/>
+      <c r="N27" s="3"/>
+      <c r="O27" s="3"/>
+      <c r="P27" s="3"/>
+      <c r="Q27" s="3"/>
+    </row>
+    <row r="28" spans="2:17">
+      <c r="B28" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6"/>
+      <c r="K28" s="6"/>
+      <c r="L28" s="6"/>
+      <c r="M28" s="6"/>
+      <c r="N28" s="3"/>
+      <c r="O28" s="3"/>
+      <c r="P28" s="3"/>
+      <c r="Q28" s="3"/>
+    </row>
+    <row r="29" spans="2:17">
+      <c r="B29" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6"/>
+      <c r="K29" s="6"/>
+      <c r="L29" s="6"/>
+      <c r="M29" s="6"/>
+      <c r="N29" s="3"/>
+      <c r="O29" s="3"/>
+      <c r="P29" s="3"/>
+      <c r="Q29" s="3"/>
+    </row>
+    <row r="30" spans="2:17" ht="43" customHeight="1">
+      <c r="B30" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="H30" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="I30" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="J30" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="K30" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="L30" s="6"/>
+      <c r="M30" s="6"/>
+      <c r="N30" s="3"/>
+      <c r="O30" s="3"/>
+      <c r="P30" s="3"/>
+      <c r="Q30" s="3"/>
+    </row>
+    <row r="31" spans="2:17">
+      <c r="B31" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="H31" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="I31" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="J31" s="8">
+        <v>130</v>
+      </c>
+      <c r="K31" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="L31" s="6"/>
+      <c r="M31" s="6"/>
+      <c r="N31" s="3"/>
+      <c r="O31" s="3"/>
+      <c r="P31" s="3"/>
+      <c r="Q31" s="3"/>
+    </row>
+    <row r="32" spans="2:17">
+      <c r="B32" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="F32" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G32" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="H32" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="I32" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="J32" s="11">
+        <v>100</v>
+      </c>
+      <c r="K32" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="L32" s="10"/>
+      <c r="M32" s="10"/>
+    </row>
+    <row r="33" spans="2:13">
+      <c r="B33" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="F33" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G33" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="H33" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="I33" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="J33" s="11">
+        <v>99</v>
+      </c>
+      <c r="K33" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="L33" s="10"/>
+      <c r="M33" s="10"/>
+    </row>
+    <row r="34" spans="2:13">
+      <c r="B34" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="F34" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G34" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="H34" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="I34" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="J34" s="11">
+        <v>70</v>
+      </c>
+      <c r="K34" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="L34" s="10"/>
+      <c r="M34" s="10"/>
+    </row>
+    <row r="35" spans="2:13" ht="43" customHeight="1">
+      <c r="B35" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="I35" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="J35" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="K35" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="L35" s="10"/>
+      <c r="M35" s="10"/>
+    </row>
+    <row r="36" spans="2:13">
+      <c r="B36" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E36" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="F36" s="11">
+        <v>150</v>
+      </c>
+      <c r="G36" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="H36" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="I36" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="J36" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="K36" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="L36" s="10"/>
+      <c r="M36" s="10"/>
+    </row>
+    <row r="37" spans="2:13">
+      <c r="B37" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="C25" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="F25" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="G25" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="H25" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="I25" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="J25" s="11">
-        <v>100</v>
-      </c>
-      <c r="K25" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="L25" s="10"/>
-      <c r="M25" s="10"/>
-    </row>
-    <row r="26" spans="2:17">
-      <c r="B26" s="9" t="s">
-        <v>175</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="E26" s="9" t="s">
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="11"/>
+      <c r="G37" s="9"/>
+      <c r="H37" s="9"/>
+      <c r="I37" s="9"/>
+      <c r="J37" s="9"/>
+      <c r="K37" s="9"/>
+      <c r="L37" s="10"/>
+      <c r="M37" s="10"/>
+    </row>
+    <row r="38" spans="2:13">
+      <c r="B38" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E38" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="F38" s="11">
+        <v>150</v>
+      </c>
+      <c r="G38" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="H38" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="I38" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="J38" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="K38" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="L38" s="10"/>
+      <c r="M38" s="10"/>
+    </row>
+    <row r="39" spans="2:13">
+      <c r="B39" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E39" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="F26" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="G26" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="H26" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="I26" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="J26" s="11">
-        <v>99</v>
-      </c>
-      <c r="K26" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="L26" s="10"/>
-      <c r="M26" s="10"/>
-    </row>
-    <row r="27" spans="2:17">
-      <c r="B27" s="9" t="s">
-        <v>176</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="E27" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="F27" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="G27" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="H27" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="I27" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="J27" s="11">
-        <v>70</v>
-      </c>
-      <c r="K27" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="L27" s="10"/>
-      <c r="M27" s="10"/>
-    </row>
-    <row r="28" spans="2:17" ht="43" customHeight="1">
-      <c r="B28" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="G28" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="H28" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="I28" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="J28" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="K28" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="L28" s="10"/>
-      <c r="M28" s="10"/>
-    </row>
-    <row r="29" spans="2:17">
-      <c r="B29" s="9" t="s">
-        <v>177</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="E29" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="F29" s="11">
-        <v>150</v>
-      </c>
-      <c r="G29" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="H29" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="I29" s="9" t="s">
+      <c r="F39" s="11">
+        <v>200</v>
+      </c>
+      <c r="G39" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="H39" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="I39" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="J29" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="K29" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="L29" s="10"/>
-      <c r="M29" s="10"/>
-    </row>
-    <row r="30" spans="2:17">
-      <c r="B30" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="D30" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="E30" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="F30" s="11">
-        <v>150</v>
-      </c>
-      <c r="G30" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="H30" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="I30" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="J30" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="K30" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="L30" s="10"/>
-      <c r="M30" s="10"/>
-    </row>
-    <row r="31" spans="2:17">
-      <c r="B31" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="E31" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="F31" s="11">
-        <v>200</v>
-      </c>
-      <c r="G31" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="H31" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="I31" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="J31" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="K31" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="L31" s="10"/>
-      <c r="M31" s="10"/>
+      <c r="J39" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="K39" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="L39" s="10"/>
+      <c r="M39" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2345,24 +2574,24 @@
   <sheetData>
     <row r="2" spans="1:4" ht="54">
       <c r="B2" s="13" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B3" s="14">
         <v>1</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D3" s="15">
         <v>1</v>
@@ -2370,13 +2599,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B4" s="14">
         <v>2</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D4" s="15">
         <v>1</v>
@@ -2384,13 +2613,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B5" s="14">
         <v>3</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="D5" s="15">
         <v>1</v>
@@ -2398,27 +2627,27 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B6" s="14">
         <v>4</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B7" s="14">
         <v>5</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D7" s="15">
         <v>1</v>
@@ -2429,7 +2658,7 @@
         <v>6</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D8" s="15">
         <v>2</v>
@@ -2440,7 +2669,7 @@
         <v>7</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="D9" s="15">
         <v>2</v>
@@ -2451,7 +2680,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="D10" s="15">
         <v>2</v>
@@ -2462,7 +2691,7 @@
         <v>9</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D11" s="15">
         <v>2</v>
@@ -2473,7 +2702,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D12" s="15">
         <v>2</v>
@@ -2484,7 +2713,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D13" s="15">
         <v>3</v>
@@ -2495,10 +2724,10 @@
         <v>12</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -2506,7 +2735,7 @@
         <v>13</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="D15" s="15">
         <v>4</v>
@@ -2517,7 +2746,7 @@
         <v>14</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="D16" s="15">
         <v>4</v>
@@ -2528,7 +2757,7 @@
         <v>15</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D17" s="15">
         <v>4</v>
@@ -2539,7 +2768,7 @@
         <v>16</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D18" s="15">
         <v>5</v>
@@ -2550,7 +2779,7 @@
         <v>17</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D19" s="15">
         <v>5</v>
@@ -2561,7 +2790,7 @@
         <v>18</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D20" s="15">
         <v>5</v>
@@ -2572,7 +2801,7 @@
         <v>19</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D21" s="15">
         <v>6</v>
@@ -2583,7 +2812,7 @@
         <v>20</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D22" s="15">
         <v>6</v>
@@ -2594,7 +2823,7 @@
         <v>21</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D23" s="15">
         <v>6</v>
@@ -2605,7 +2834,7 @@
         <v>22</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D24" s="15">
         <v>7</v>
@@ -2616,7 +2845,7 @@
         <v>23</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="D25" s="15">
         <v>7</v>
@@ -2627,7 +2856,7 @@
         <v>24</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D26" s="15">
         <v>7</v>
@@ -2638,7 +2867,7 @@
         <v>25</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="D27" s="15">
         <v>7</v>
@@ -2646,7 +2875,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
added more smart watches to the tech table
</commit_message>
<xml_diff>
--- a/Documentations/Features-Garrett.xlsx
+++ b/Documentations/Features-Garrett.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="200" yWindow="280" windowWidth="14380" windowHeight="16640" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="680" yWindow="680" windowWidth="28800" windowHeight="17480" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="196">
   <si>
     <t>REQUIRED</t>
   </si>
@@ -561,6 +561,54 @@
   </si>
   <si>
     <t>Mio Alpha [18]</t>
+  </si>
+  <si>
+    <t>Touch Screen</t>
+  </si>
+  <si>
+    <t>Battery Life</t>
+  </si>
+  <si>
+    <t>Solar powered</t>
+  </si>
+  <si>
+    <t>3-4 days</t>
+  </si>
+  <si>
+    <t>2 years</t>
+  </si>
+  <si>
+    <t>2 days</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>7 days</t>
+  </si>
+  <si>
+    <t>BT &amp; Wi-Fi</t>
+  </si>
+  <si>
+    <t>LED</t>
+  </si>
+  <si>
+    <t>Basis B1 [B4]</t>
+  </si>
+  <si>
+    <t>Casio G-Shock GB-6900 [B5]</t>
+  </si>
+  <si>
+    <t>Citizen Eco-drive Proximity [B10]</t>
+  </si>
+  <si>
+    <t>WIMM One [B8]</t>
+  </si>
+  <si>
+    <t>Dial</t>
+  </si>
+  <si>
+    <t>8-10 hours</t>
   </si>
 </sst>
 </file>
@@ -659,7 +707,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -682,8 +730,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="47">
+  <cellStyleXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -731,8 +790,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -777,8 +842,15 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="47">
+  <cellStyles count="53">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -802,6 +874,9 @@
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -825,6 +900,9 @@
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1325,7 +1403,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1336,10 +1413,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:Q31"/>
+  <dimension ref="B4:Q35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="M35" sqref="B28:M35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2211,8 +2288,12 @@
       <c r="K28" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="L28" s="10"/>
-      <c r="M28" s="10"/>
+      <c r="L28" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="M28" s="10" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="29" spans="2:17">
       <c r="B29" s="9" t="s">
@@ -2245,8 +2326,12 @@
       <c r="K29" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="L29" s="10"/>
-      <c r="M29" s="10"/>
+      <c r="L29" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="M29" s="10" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="30" spans="2:17">
       <c r="B30" s="9" t="s">
@@ -2279,8 +2364,12 @@
       <c r="K30" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="L30" s="10"/>
-      <c r="M30" s="10"/>
+      <c r="L30" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="M30" s="10" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="31" spans="2:17">
       <c r="B31" s="9" t="s">
@@ -2313,8 +2402,164 @@
       <c r="K31" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="L31" s="10"/>
-      <c r="M31" s="10"/>
+      <c r="L31" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="M31" s="10" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="32" spans="2:17">
+      <c r="B32" t="s">
+        <v>190</v>
+      </c>
+      <c r="C32" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="D32" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="E32" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="F32" s="18">
+        <v>199</v>
+      </c>
+      <c r="G32" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="H32" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="I32" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="J32" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="K32" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="L32" t="s">
+        <v>42</v>
+      </c>
+      <c r="M32" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="33" spans="2:13">
+      <c r="B33" t="s">
+        <v>191</v>
+      </c>
+      <c r="C33" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="D33" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="E33" s="20" t="s">
+        <v>189</v>
+      </c>
+      <c r="F33" s="18">
+        <v>180</v>
+      </c>
+      <c r="G33" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="H33" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="I33" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="J33" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="K33" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="L33" t="s">
+        <v>42</v>
+      </c>
+      <c r="M33" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="34" spans="2:13">
+      <c r="B34" t="s">
+        <v>192</v>
+      </c>
+      <c r="C34" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="D34" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="E34" s="20" t="s">
+        <v>194</v>
+      </c>
+      <c r="F34" s="18">
+        <v>345</v>
+      </c>
+      <c r="G34" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="H34" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="I34" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="J34" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="K34" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="L34" t="s">
+        <v>42</v>
+      </c>
+      <c r="M34" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="35" spans="2:13">
+      <c r="B35" t="s">
+        <v>193</v>
+      </c>
+      <c r="C35" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="D35" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="E35" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="F35" s="18">
+        <v>200</v>
+      </c>
+      <c r="G35" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="H35" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="I35" s="19" t="s">
+        <v>188</v>
+      </c>
+      <c r="J35" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="K35" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="L35" t="s">
+        <v>43</v>
+      </c>
+      <c r="M35" t="s">
+        <v>185</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -2646,7 +2891,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
added watches to tech table after git pooped on itself and forced me to delete it
</commit_message>
<xml_diff>
--- a/Documentations/Features-Garrett.xlsx
+++ b/Documentations/Features-Garrett.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="208">
   <si>
     <t>REQUIRED</t>
   </si>
@@ -545,9 +545,6 @@
     <t>Mio Alpha [18]</t>
   </si>
   <si>
-    <t>Samasung Galaxy Gear</t>
-  </si>
-  <si>
     <t>Phone (Android)</t>
   </si>
   <si>
@@ -600,6 +597,54 @@
   </si>
   <si>
     <t>Yes (some)</t>
+  </si>
+  <si>
+    <t>Touch Screen</t>
+  </si>
+  <si>
+    <t>Battery Life</t>
+  </si>
+  <si>
+    <t>7 days</t>
+  </si>
+  <si>
+    <t>3-4 days</t>
+  </si>
+  <si>
+    <t>8-10 hours</t>
+  </si>
+  <si>
+    <t>Basis B1 [B4]</t>
+  </si>
+  <si>
+    <t>Casio G-Shock GB-6900 [B5]</t>
+  </si>
+  <si>
+    <t>LED</t>
+  </si>
+  <si>
+    <t>2 years</t>
+  </si>
+  <si>
+    <t>Citizen Eco-drive Proximity [B10]</t>
+  </si>
+  <si>
+    <t>Dial</t>
+  </si>
+  <si>
+    <t>Solar powered</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>WIMM One [B8]</t>
+  </si>
+  <si>
+    <t>BT &amp; Wi-Fi</t>
+  </si>
+  <si>
+    <t>2 days</t>
   </si>
 </sst>
 </file>
@@ -698,7 +743,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -719,6 +764,17 @@
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -771,7 +827,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -814,6 +870,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1374,10 +1437,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:Q39"/>
+  <dimension ref="B4:Q42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" topLeftCell="B23" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1428,7 +1491,7 @@
     </row>
     <row r="5" spans="2:17">
       <c r="B5" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>42</v>
@@ -1458,7 +1521,7 @@
     </row>
     <row r="6" spans="2:17">
       <c r="B6" s="6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>41</v>
@@ -1500,7 +1563,7 @@
         <v>53</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>55</v>
@@ -1557,7 +1620,7 @@
         <v>54</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="L8" s="6" t="s">
         <v>42</v>
@@ -1614,13 +1677,13 @@
     </row>
     <row r="10" spans="2:17">
       <c r="B10" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>41</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>41</v>
@@ -1629,7 +1692,7 @@
         <v>41</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -1648,14 +1711,14 @@
     </row>
     <row r="11" spans="2:17">
       <c r="B11" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>187</v>
-      </c>
       <c r="E11" s="6" t="s">
         <v>42</v>
       </c>
@@ -1663,7 +1726,7 @@
         <v>41</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -1673,7 +1736,7 @@
         <v>41</v>
       </c>
       <c r="M11" s="6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="N11" s="3"/>
       <c r="O11" s="3"/>
@@ -1682,7 +1745,7 @@
     </row>
     <row r="12" spans="2:17">
       <c r="B12" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>41</v>
@@ -1992,7 +2055,7 @@
     </row>
     <row r="21" spans="2:17">
       <c r="B21" s="6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
@@ -2102,7 +2165,7 @@
     </row>
     <row r="25" spans="2:17">
       <c r="B25" s="6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
@@ -2122,7 +2185,7 @@
     </row>
     <row r="26" spans="2:17">
       <c r="B26" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>42</v>
@@ -2150,7 +2213,7 @@
     </row>
     <row r="27" spans="2:17">
       <c r="B27" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>42</v>
@@ -2178,7 +2241,7 @@
     </row>
     <row r="28" spans="2:17">
       <c r="B28" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
@@ -2198,7 +2261,7 @@
     </row>
     <row r="29" spans="2:17">
       <c r="B29" s="6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
@@ -2425,8 +2488,12 @@
       <c r="K35" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="L35" s="10"/>
-      <c r="M35" s="10"/>
+      <c r="L35" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="M35" s="10" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="36" spans="2:13">
       <c r="B36" s="9" t="s">
@@ -2459,40 +2526,66 @@
       <c r="K36" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="L36" s="10"/>
-      <c r="M36" s="10"/>
+      <c r="L36" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="M36" s="10" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="37" spans="2:13">
       <c r="B37" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="C37" s="9"/>
-      <c r="D37" s="9"/>
-      <c r="E37" s="9"/>
-      <c r="F37" s="11"/>
-      <c r="G37" s="9"/>
-      <c r="H37" s="9"/>
-      <c r="I37" s="9"/>
-      <c r="J37" s="9"/>
-      <c r="K37" s="9"/>
-      <c r="L37" s="10"/>
-      <c r="M37" s="10"/>
+        <v>172</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E37" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="F37" s="11">
+        <v>150</v>
+      </c>
+      <c r="G37" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="H37" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="I37" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="J37" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="K37" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="L37" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="M37" s="10" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="38" spans="2:13">
       <c r="B38" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>41</v>
+        <v>117</v>
       </c>
       <c r="D38" s="9" t="s">
         <v>41</v>
       </c>
       <c r="E38" s="9" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="F38" s="11">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="G38" s="9" t="s">
         <v>41</v>
@@ -2507,44 +2600,166 @@
         <v>42</v>
       </c>
       <c r="K38" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="L38" s="10"/>
-      <c r="M38" s="10"/>
+        <v>42</v>
+      </c>
+      <c r="L38" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="M38" s="10" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="39" spans="2:13">
-      <c r="B39" s="9" t="s">
-        <v>173</v>
-      </c>
-      <c r="C39" s="9" t="s">
+      <c r="B39" t="s">
+        <v>197</v>
+      </c>
+      <c r="C39" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="D39" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="E39" s="9" t="s">
+      <c r="D39" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="E39" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="F39" s="11">
+      <c r="F39" s="19">
+        <v>199</v>
+      </c>
+      <c r="G39" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="H39" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="I39" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="J39" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="K39" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="L39" t="s">
+        <v>41</v>
+      </c>
+      <c r="M39" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="40" spans="2:13">
+      <c r="B40" t="s">
+        <v>198</v>
+      </c>
+      <c r="C40" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="D40" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="E40" s="18" t="s">
+        <v>199</v>
+      </c>
+      <c r="F40" s="19">
+        <v>180</v>
+      </c>
+      <c r="G40" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="H40" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="I40" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="J40" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="K40" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="L40" t="s">
+        <v>41</v>
+      </c>
+      <c r="M40" t="s">
         <v>200</v>
       </c>
-      <c r="G39" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="H39" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="I39" s="9" t="s">
+    </row>
+    <row r="41" spans="2:13">
+      <c r="B41" t="s">
+        <v>201</v>
+      </c>
+      <c r="C41" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="D41" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="E41" s="18" t="s">
+        <v>202</v>
+      </c>
+      <c r="F41" s="19">
+        <v>345</v>
+      </c>
+      <c r="G41" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="H41" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="I41" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="J39" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="K39" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="L39" s="10"/>
-      <c r="M39" s="10"/>
+      <c r="J41" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="K41" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="L41" t="s">
+        <v>41</v>
+      </c>
+      <c r="M41" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="42" spans="2:13">
+      <c r="B42" t="s">
+        <v>205</v>
+      </c>
+      <c r="C42" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="D42" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="E42" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="F42" s="19">
+        <v>200</v>
+      </c>
+      <c r="G42" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="H42" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="I42" s="20" t="s">
+        <v>206</v>
+      </c>
+      <c r="J42" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="K42" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="L42" t="s">
+        <v>42</v>
+      </c>
+      <c r="M42" t="s">
+        <v>207</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
updated the tech table
</commit_message>
<xml_diff>
--- a/Documentations/Features-Garrett.xlsx
+++ b/Documentations/Features-Garrett.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="216">
   <si>
     <t>REQUIRED</t>
   </si>
@@ -645,6 +645,30 @@
   </si>
   <si>
     <t>2 days</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>250 kb/s</t>
+  </si>
+  <si>
+    <t>up to 100m</t>
+  </si>
+  <si>
+    <t>low</t>
+  </si>
+  <si>
+    <t>15v or 5v</t>
+  </si>
+  <si>
+    <t>.05 uA / cm^2</t>
+  </si>
+  <si>
+    <t>integrated driver</t>
+  </si>
+  <si>
+    <t>varies</t>
   </si>
 </sst>
 </file>
@@ -1439,8 +1463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:Q42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B23" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1694,10 +1718,18 @@
       <c r="G10" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
+      <c r="H10" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="K10" s="6" t="s">
+        <v>68</v>
+      </c>
       <c r="L10" s="6" t="s">
         <v>42</v>
       </c>
@@ -1728,10 +1760,18 @@
       <c r="G11" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
+      <c r="H11" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="K11" s="6" t="s">
+        <v>187</v>
+      </c>
       <c r="L11" s="6" t="s">
         <v>41</v>
       </c>
@@ -1750,16 +1790,30 @@
       <c r="C12" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
+      <c r="D12" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>208</v>
+      </c>
       <c r="F12" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
+      <c r="G12" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>211</v>
+      </c>
       <c r="L12" s="6" t="s">
         <v>41</v>
       </c>
@@ -2053,17 +2107,31 @@
       <c r="P20" s="3"/>
       <c r="Q20" s="3"/>
     </row>
-    <row r="21" spans="2:17">
+    <row r="21" spans="2:17" ht="30">
       <c r="B21" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
+      <c r="C21" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="I21" s="6" t="s">
+        <v>215</v>
+      </c>
       <c r="J21" s="6"/>
       <c r="K21" s="6"/>
       <c r="L21" s="6"/>
@@ -2167,10 +2235,18 @@
       <c r="B25" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
+      <c r="C25" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>41</v>
+      </c>
       <c r="G25" s="6"/>
       <c r="H25" s="6"/>
       <c r="I25" s="6"/>
@@ -2191,10 +2267,10 @@
         <v>42</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F26" s="6" t="s">
         <v>42</v>
@@ -2243,10 +2319,18 @@
       <c r="B28" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
+      <c r="C28" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>42</v>
+      </c>
       <c r="G28" s="6"/>
       <c r="H28" s="6"/>
       <c r="I28" s="6"/>
@@ -2263,10 +2347,18 @@
       <c r="B29" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
+      <c r="C29" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>41</v>
+      </c>
       <c r="G29" s="6"/>
       <c r="H29" s="6"/>
       <c r="I29" s="6"/>

</xml_diff>

<commit_message>
gave each of us folders to keep our individual docs in so others can view them. probably best if we don't modify eachothers documents
</commit_message>
<xml_diff>
--- a/Documentations/Features-Garrett.xlsx
+++ b/Documentations/Features-Garrett.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
-  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
+  <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="200" yWindow="280" windowWidth="26780" windowHeight="16640" tabRatio="500" activeTab="1"/>
   </bookViews>
@@ -11,6 +11,9 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Sheet2!$B$4:$M$42</definedName>
+  </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -767,7 +770,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -788,17 +791,6 @@
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -851,7 +843,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -896,13 +888,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="47">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1450,7 +1436,9 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1463,8 +1451,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:Q42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4:M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1502,12 +1490,12 @@
       <c r="G4" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
       <c r="P4" s="3"/>
@@ -1853,9 +1841,9 @@
       <c r="J13" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6"/>
-      <c r="M13" s="6"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
       <c r="N13" s="3"/>
       <c r="O13" s="3"/>
       <c r="P13" s="3"/>
@@ -2030,10 +2018,10 @@
       <c r="I18" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="J18" s="6"/>
-      <c r="K18" s="6"/>
-      <c r="L18" s="6"/>
-      <c r="M18" s="6"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
       <c r="N18" s="3"/>
       <c r="O18" s="3"/>
       <c r="P18" s="3"/>
@@ -2191,13 +2179,13 @@
       <c r="F23" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
-      <c r="K23" s="6"/>
-      <c r="L23" s="6"/>
-      <c r="M23" s="6"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
       <c r="N23" s="3"/>
       <c r="O23" s="3"/>
       <c r="P23" s="3"/>
@@ -2402,8 +2390,8 @@
       <c r="K30" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="L30" s="6"/>
-      <c r="M30" s="6"/>
+      <c r="L30" s="5"/>
+      <c r="M30" s="5"/>
       <c r="N30" s="3"/>
       <c r="O30" s="3"/>
       <c r="P30" s="3"/>
@@ -2580,10 +2568,10 @@
       <c r="K35" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="L35" s="10" t="s">
+      <c r="L35" s="18" t="s">
         <v>192</v>
       </c>
-      <c r="M35" s="10" t="s">
+      <c r="M35" s="18" t="s">
         <v>193</v>
       </c>
     </row>
@@ -2702,160 +2690,168 @@
       </c>
     </row>
     <row r="39" spans="2:13">
-      <c r="B39" t="s">
+      <c r="B39" s="10" t="s">
         <v>197</v>
       </c>
-      <c r="C39" s="18" t="s">
+      <c r="C39" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="D39" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="E39" s="18" t="s">
+      <c r="D39" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E39" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="F39" s="19">
+      <c r="F39" s="11">
         <v>199</v>
       </c>
-      <c r="G39" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="H39" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="I39" s="18" t="s">
+      <c r="G39" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="H39" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="I39" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="J39" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="K39" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="L39" t="s">
-        <v>41</v>
-      </c>
-      <c r="M39" t="s">
+      <c r="J39" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="K39" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="L39" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="M39" s="10" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="40" spans="2:13">
-      <c r="B40" t="s">
+      <c r="B40" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="C40" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="D40" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="E40" s="18" t="s">
+      <c r="C40" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E40" s="9" t="s">
         <v>199</v>
       </c>
-      <c r="F40" s="19">
+      <c r="F40" s="11">
         <v>180</v>
       </c>
-      <c r="G40" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="H40" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="I40" s="18" t="s">
+      <c r="G40" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="H40" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="I40" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="J40" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="K40" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="L40" t="s">
-        <v>41</v>
-      </c>
-      <c r="M40" t="s">
+      <c r="J40" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="K40" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="L40" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="M40" s="10" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="41" spans="2:13">
-      <c r="B41" t="s">
+      <c r="B41" s="10" t="s">
         <v>201</v>
       </c>
-      <c r="C41" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="D41" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="E41" s="18" t="s">
+      <c r="C41" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E41" s="9" t="s">
         <v>202</v>
       </c>
-      <c r="F41" s="19">
+      <c r="F41" s="11">
         <v>345</v>
       </c>
-      <c r="G41" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="H41" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="I41" s="18" t="s">
+      <c r="G41" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="H41" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="I41" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="J41" s="20" t="s">
+      <c r="J41" s="9" t="s">
         <v>203</v>
       </c>
-      <c r="K41" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="L41" t="s">
-        <v>41</v>
-      </c>
-      <c r="M41" t="s">
+      <c r="K41" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="L41" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="M41" s="10" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="42" spans="2:13">
-      <c r="B42" t="s">
+      <c r="B42" s="10" t="s">
         <v>205</v>
       </c>
-      <c r="C42" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="D42" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="E42" s="18" t="s">
+      <c r="C42" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E42" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="F42" s="19">
+      <c r="F42" s="11">
         <v>200</v>
       </c>
-      <c r="G42" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="H42" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="I42" s="20" t="s">
+      <c r="G42" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="H42" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="I42" s="9" t="s">
         <v>206</v>
       </c>
-      <c r="J42" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="K42" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="L42" t="s">
-        <v>42</v>
-      </c>
-      <c r="M42" t="s">
+      <c r="J42" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="K42" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="L42" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="M42" s="10" t="s">
         <v>207</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="60" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <rowBreaks count="1" manualBreakCount="1">
+    <brk id="42" max="16383" man="1"/>
+  </rowBreaks>
+  <colBreaks count="2" manualBreakCount="2">
+    <brk id="1" max="1048575" man="1"/>
+    <brk id="13" max="1048575" man="1"/>
+  </colBreaks>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3181,7 +3177,9 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>